<commit_message>
Made corrections for Rev2 PCB
Plating on both sides of battery slots, internal clearance on same net components (GND) and naming.
</commit_message>
<xml_diff>
--- a/P80/BP8/Rev2/PCB_ordering_document.xlsx
+++ b/P80/BP8/Rev2/PCB_ordering_document.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="Denne_projektmappe" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mogn\Documents\GitHub\Hardware\nanopower\P80\BalancedBatteryPack\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Mogn\Documents\GitHub\Hardware\nanopower\P80\BP8\Rev3\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9516" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9516"/>
   </bookViews>
   <sheets>
     <sheet name="PCB Specifications" sheetId="1" r:id="rId1"/>
@@ -1269,109 +1269,149 @@
     <xf numFmtId="0" fontId="5" fillId="6" borderId="14" xfId="3" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="13" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="13" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+      <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="15" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1417,26 +1457,89 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="16" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
@@ -1444,135 +1547,32 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="2"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="35" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="1" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="15" xfId="6" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="2"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="22" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="14" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="4" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="15" xfId="5" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="21" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="13" borderId="26" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="26" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="13" borderId="22" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="7">
@@ -3053,8 +3053,8 @@
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>41</xdr:row>
-          <xdr:rowOff>185530</xdr:rowOff>
+          <xdr:row>42</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3187,8 +3187,8 @@
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>41</xdr:row>
-          <xdr:rowOff>185530</xdr:rowOff>
+          <xdr:row>42</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3254,8 +3254,8 @@
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>41</xdr:row>
-          <xdr:rowOff>185530</xdr:rowOff>
+          <xdr:row>42</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3322,7 +3322,7 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>43</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3791,7 +3791,7 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>50</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3925,7 +3925,7 @@
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
           <xdr:row>50</xdr:row>
-          <xdr:rowOff>1</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -3991,8 +3991,8 @@
         <xdr:to>
           <xdr:col>2</xdr:col>
           <xdr:colOff>0</xdr:colOff>
-          <xdr:row>50</xdr:row>
-          <xdr:rowOff>190500</xdr:rowOff>
+          <xdr:row>51</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -4186,7 +4186,7 @@
                   <a14:compatExt spid="_x0000_s1066"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{96B840C5-22A5-4718-8C70-F516685B3D01}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002A040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4232,14 +4232,19 @@
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>175260</xdr:colOff>
           <xdr:row>38</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="447592" cy="185530"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>39</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1067" name="Check Box 43" hidden="1">
@@ -4248,7 +4253,7 @@
                   <a14:compatExt spid="_x0000_s1067"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{154AD7D6-90C6-43A8-BF14-B0DB0E8BF3EC}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002B040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4288,20 +4293,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>175260</xdr:colOff>
           <xdr:row>38</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="447592" cy="185531"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>39</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1068" name="Check Box 44" hidden="1">
@@ -4310,7 +4320,7 @@
                   <a14:compatExt spid="_x0000_s1068"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{84468357-637C-4B0A-B7AD-AFC8177F5E9B}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002C040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4350,20 +4360,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>175260</xdr:colOff>
           <xdr:row>38</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="447592" cy="185530"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>39</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1069" name="Check Box 45" hidden="1">
@@ -4372,7 +4387,7 @@
                   <a14:compatExt spid="_x0000_s1069"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{440AB5FF-8598-4EE3-9502-281A490A16C5}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002D040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4412,20 +4427,25 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
-      <xdr:oneCellAnchor>
+      <xdr:twoCellAnchor editAs="oneCell">
         <xdr:from>
           <xdr:col>1</xdr:col>
           <xdr:colOff>175260</xdr:colOff>
           <xdr:row>37</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:from>
-        <xdr:ext cx="447592" cy="185531"/>
+        <xdr:to>
+          <xdr:col>2</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>38</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="1070" name="Check Box 46" hidden="1">
@@ -4434,7 +4454,7 @@
                   <a14:compatExt spid="_x0000_s1070"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F8F959C0-0D67-44BE-982D-1803256F9249}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002E040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4474,7 +4494,7 @@
           </xdr:spPr>
         </xdr:sp>
         <xdr:clientData/>
-      </xdr:oneCellAnchor>
+      </xdr:twoCellAnchor>
     </mc:Choice>
     <mc:Fallback/>
   </mc:AlternateContent>
@@ -4501,7 +4521,7 @@
                   <a14:compatExt spid="_x0000_s1071"/>
                 </a:ext>
                 <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{72821675-3124-483A-B2B7-AFD7C07B01D4}"/>
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-00002F040000}"/>
                 </a:ext>
               </a:extLst>
             </xdr:cNvPr>
@@ -4874,8 +4894,8 @@
   </sheetPr>
   <dimension ref="A1:O333"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -4894,222 +4914,222 @@
   <sheetData>
     <row r="1" spans="2:8" s="9" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="2" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B2" s="94" t="s">
+      <c r="B2" s="142" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="95"/>
-      <c r="D2" s="96"/>
+      <c r="C2" s="143"/>
+      <c r="D2" s="144"/>
       <c r="E2" s="22"/>
       <c r="F2" s="21"/>
-      <c r="G2" s="89"/>
-      <c r="H2" s="90"/>
+      <c r="G2" s="139"/>
+      <c r="H2" s="140"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B3" s="97" t="s">
+      <c r="B3" s="145" t="s">
         <v>80</v>
       </c>
-      <c r="C3" s="98"/>
-      <c r="D3" s="99"/>
+      <c r="C3" s="146"/>
+      <c r="D3" s="147"/>
       <c r="E3" s="23"/>
       <c r="F3" s="18"/>
-      <c r="G3" s="91"/>
-      <c r="H3" s="92"/>
+      <c r="G3" s="121"/>
+      <c r="H3" s="141"/>
     </row>
     <row r="4" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="100" t="s">
+      <c r="B4" s="148" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="101"/>
-      <c r="D4" s="102"/>
+      <c r="C4" s="149"/>
+      <c r="D4" s="150"/>
       <c r="E4" s="23"/>
       <c r="F4" s="18"/>
-      <c r="G4" s="91"/>
-      <c r="H4" s="92"/>
+      <c r="G4" s="121"/>
+      <c r="H4" s="141"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B5" s="100" t="s">
+      <c r="B5" s="148" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="101"/>
-      <c r="D5" s="102"/>
+      <c r="C5" s="149"/>
+      <c r="D5" s="150"/>
       <c r="E5" s="23"/>
       <c r="F5" s="18"/>
-      <c r="G5" s="91"/>
-      <c r="H5" s="92"/>
+      <c r="G5" s="121"/>
+      <c r="H5" s="141"/>
     </row>
     <row r="6" spans="2:8" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="103" t="s">
+      <c r="B6" s="151" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="104"/>
-      <c r="D6" s="105"/>
+      <c r="C6" s="152"/>
+      <c r="D6" s="153"/>
       <c r="E6" s="25"/>
       <c r="F6" s="26"/>
       <c r="G6" s="26"/>
       <c r="H6" s="27"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="106"/>
-      <c r="C7" s="107"/>
-      <c r="D7" s="107"/>
-      <c r="E7" s="107"/>
-      <c r="F7" s="107"/>
-      <c r="G7" s="107"/>
-      <c r="H7" s="108"/>
+      <c r="B7" s="154"/>
+      <c r="C7" s="155"/>
+      <c r="D7" s="155"/>
+      <c r="E7" s="155"/>
+      <c r="F7" s="155"/>
+      <c r="G7" s="155"/>
+      <c r="H7" s="156"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B8" s="88"/>
-      <c r="C8" s="109" t="s">
+      <c r="B8" s="160"/>
+      <c r="C8" s="92" t="s">
         <v>13</v>
       </c>
-      <c r="D8" s="123"/>
-      <c r="E8" s="123"/>
-      <c r="F8" s="124"/>
-      <c r="G8" s="142">
+      <c r="D8" s="93"/>
+      <c r="E8" s="93"/>
+      <c r="F8" s="94"/>
+      <c r="G8" s="98">
         <f ca="1">TODAY()</f>
-        <v>43076</v>
-      </c>
-      <c r="H8" s="84"/>
+        <v>43108</v>
+      </c>
+      <c r="H8" s="99"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B9" s="88"/>
-      <c r="C9" s="144" t="s">
+      <c r="B9" s="160"/>
+      <c r="C9" s="95" t="s">
         <v>1</v>
       </c>
-      <c r="D9" s="145"/>
-      <c r="E9" s="145"/>
-      <c r="F9" s="146"/>
-      <c r="G9" s="125" t="s">
+      <c r="D9" s="96"/>
+      <c r="E9" s="96"/>
+      <c r="F9" s="97"/>
+      <c r="G9" s="100" t="s">
         <v>88</v>
       </c>
-      <c r="H9" s="143"/>
+      <c r="H9" s="101"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B10" s="88"/>
-      <c r="C10" s="109" t="s">
+      <c r="B10" s="160"/>
+      <c r="C10" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="123"/>
-      <c r="E10" s="123"/>
-      <c r="F10" s="124"/>
-      <c r="G10" s="79">
+      <c r="D10" s="93"/>
+      <c r="E10" s="93"/>
+      <c r="F10" s="94"/>
+      <c r="G10" s="102">
         <v>100386</v>
       </c>
-      <c r="H10" s="84"/>
+      <c r="H10" s="99"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B11" s="88"/>
-      <c r="C11" s="144" t="s">
+      <c r="B11" s="160"/>
+      <c r="C11" s="95" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="145"/>
-      <c r="E11" s="145"/>
-      <c r="F11" s="146"/>
-      <c r="G11" s="125">
-        <v>1</v>
-      </c>
-      <c r="H11" s="143"/>
+      <c r="D11" s="96"/>
+      <c r="E11" s="96"/>
+      <c r="F11" s="97"/>
+      <c r="G11" s="100">
+        <v>2</v>
+      </c>
+      <c r="H11" s="101"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B12" s="88"/>
-      <c r="C12" s="109" t="s">
+      <c r="B12" s="160"/>
+      <c r="C12" s="92" t="s">
         <v>3</v>
       </c>
-      <c r="D12" s="123"/>
-      <c r="E12" s="123"/>
-      <c r="F12" s="124"/>
-      <c r="G12" s="79" t="s">
+      <c r="D12" s="93"/>
+      <c r="E12" s="93"/>
+      <c r="F12" s="94"/>
+      <c r="G12" s="102" t="s">
         <v>89</v>
       </c>
-      <c r="H12" s="84"/>
+      <c r="H12" s="99"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B13" s="88"/>
-      <c r="C13" s="81" t="s">
+      <c r="B13" s="160"/>
+      <c r="C13" s="158" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="81"/>
-      <c r="E13" s="81"/>
-      <c r="F13" s="81"/>
-      <c r="G13" s="81"/>
-      <c r="H13" s="82"/>
+      <c r="D13" s="158"/>
+      <c r="E13" s="158"/>
+      <c r="F13" s="158"/>
+      <c r="G13" s="158"/>
+      <c r="H13" s="159"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B14" s="88"/>
-      <c r="C14" s="79" t="s">
+      <c r="B14" s="160"/>
+      <c r="C14" s="102" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="79"/>
-      <c r="E14" s="79"/>
-      <c r="F14" s="79"/>
-      <c r="G14" s="79" t="s">
+      <c r="D14" s="102"/>
+      <c r="E14" s="102"/>
+      <c r="F14" s="102"/>
+      <c r="G14" s="102" t="s">
         <v>79</v>
       </c>
-      <c r="H14" s="84"/>
+      <c r="H14" s="99"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B15" s="88"/>
-      <c r="C15" s="80" t="s">
+      <c r="B15" s="160"/>
+      <c r="C15" s="105" t="s">
         <v>31</v>
       </c>
-      <c r="D15" s="80"/>
-      <c r="E15" s="80"/>
-      <c r="F15" s="80"/>
-      <c r="G15" s="80" t="s">
+      <c r="D15" s="105"/>
+      <c r="E15" s="105"/>
+      <c r="F15" s="105"/>
+      <c r="G15" s="105" t="s">
         <v>81</v>
       </c>
-      <c r="H15" s="83"/>
+      <c r="H15" s="106"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.3">
-      <c r="B16" s="88"/>
-      <c r="C16" s="79" t="s">
+      <c r="B16" s="160"/>
+      <c r="C16" s="102" t="s">
         <v>30</v>
       </c>
-      <c r="D16" s="79"/>
-      <c r="E16" s="79"/>
-      <c r="F16" s="79"/>
-      <c r="G16" s="79" t="s">
+      <c r="D16" s="102"/>
+      <c r="E16" s="102"/>
+      <c r="F16" s="102"/>
+      <c r="G16" s="102" t="s">
         <v>32</v>
       </c>
-      <c r="H16" s="84"/>
+      <c r="H16" s="99"/>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B17" s="88"/>
-      <c r="C17" s="80" t="s">
+      <c r="B17" s="160"/>
+      <c r="C17" s="105" t="s">
         <v>24</v>
       </c>
-      <c r="D17" s="80"/>
-      <c r="E17" s="80"/>
-      <c r="F17" s="80"/>
-      <c r="G17" s="80">
+      <c r="D17" s="105"/>
+      <c r="E17" s="105"/>
+      <c r="F17" s="105"/>
+      <c r="G17" s="105">
         <v>8</v>
       </c>
-      <c r="H17" s="83"/>
+      <c r="H17" s="106"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B18" s="88"/>
-      <c r="C18" s="79" t="s">
+      <c r="B18" s="160"/>
+      <c r="C18" s="102" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="79"/>
-      <c r="E18" s="79"/>
-      <c r="F18" s="79"/>
-      <c r="G18" s="140" t="s">
+      <c r="D18" s="102"/>
+      <c r="E18" s="102"/>
+      <c r="F18" s="102"/>
+      <c r="G18" s="103" t="s">
         <v>66</v>
       </c>
-      <c r="H18" s="141"/>
+      <c r="H18" s="104"/>
     </row>
     <row r="19" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="16"/>
-      <c r="B19" s="85" t="s">
+      <c r="B19" s="107" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="86"/>
-      <c r="D19" s="86"/>
-      <c r="E19" s="86"/>
-      <c r="F19" s="86"/>
-      <c r="G19" s="86"/>
-      <c r="H19" s="87"/>
+      <c r="C19" s="108"/>
+      <c r="D19" s="108"/>
+      <c r="E19" s="108"/>
+      <c r="F19" s="108"/>
+      <c r="G19" s="108"/>
+      <c r="H19" s="109"/>
       <c r="I19" s="16"/>
       <c r="J19" s="16"/>
       <c r="K19" s="16"/>
@@ -5121,16 +5141,16 @@
     <row r="20" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="16"/>
       <c r="B20" s="2"/>
-      <c r="C20" s="79" t="s">
+      <c r="C20" s="102" t="s">
         <v>26</v>
       </c>
-      <c r="D20" s="79"/>
-      <c r="E20" s="79"/>
-      <c r="F20" s="79"/>
-      <c r="G20" s="79" t="s">
+      <c r="D20" s="102"/>
+      <c r="E20" s="102"/>
+      <c r="F20" s="102"/>
+      <c r="G20" s="102" t="s">
         <v>28</v>
       </c>
-      <c r="H20" s="84"/>
+      <c r="H20" s="99"/>
       <c r="I20" s="16"/>
       <c r="J20" s="16"/>
       <c r="K20" s="16"/>
@@ -5142,16 +5162,16 @@
     <row r="21" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="16"/>
       <c r="B21" s="1"/>
-      <c r="C21" s="80" t="s">
+      <c r="C21" s="105" t="s">
         <v>27</v>
       </c>
-      <c r="D21" s="80"/>
-      <c r="E21" s="80"/>
-      <c r="F21" s="80"/>
-      <c r="G21" s="80" t="s">
+      <c r="D21" s="105"/>
+      <c r="E21" s="105"/>
+      <c r="F21" s="105"/>
+      <c r="G21" s="105" t="s">
         <v>28</v>
       </c>
-      <c r="H21" s="83"/>
+      <c r="H21" s="106"/>
       <c r="I21" s="16"/>
       <c r="J21" s="16"/>
       <c r="K21" s="16"/>
@@ -5163,16 +5183,16 @@
     <row r="22" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="16"/>
       <c r="B22" s="2"/>
-      <c r="C22" s="79" t="s">
+      <c r="C22" s="102" t="s">
         <v>76</v>
       </c>
-      <c r="D22" s="79"/>
-      <c r="E22" s="79"/>
-      <c r="F22" s="79"/>
-      <c r="G22" s="79" t="s">
+      <c r="D22" s="102"/>
+      <c r="E22" s="102"/>
+      <c r="F22" s="102"/>
+      <c r="G22" s="102" t="s">
         <v>73</v>
       </c>
-      <c r="H22" s="84"/>
+      <c r="H22" s="99"/>
       <c r="I22" s="16"/>
       <c r="J22" s="16"/>
       <c r="K22" s="16"/>
@@ -5184,16 +5204,16 @@
     <row r="23" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="16"/>
       <c r="B23" s="1"/>
-      <c r="C23" s="80" t="s">
+      <c r="C23" s="105" t="s">
         <v>82</v>
       </c>
-      <c r="D23" s="80"/>
-      <c r="E23" s="80"/>
-      <c r="F23" s="80"/>
-      <c r="G23" s="80" t="s">
+      <c r="D23" s="105"/>
+      <c r="E23" s="105"/>
+      <c r="F23" s="105"/>
+      <c r="G23" s="105" t="s">
         <v>83</v>
       </c>
-      <c r="H23" s="83"/>
+      <c r="H23" s="106"/>
       <c r="I23" s="16"/>
       <c r="J23" s="16"/>
       <c r="K23" s="16"/>
@@ -5205,16 +5225,16 @@
     <row r="24" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="16"/>
       <c r="B24" s="2"/>
-      <c r="C24" s="79" t="s">
+      <c r="C24" s="102" t="s">
         <v>29</v>
       </c>
-      <c r="D24" s="79"/>
-      <c r="E24" s="79"/>
-      <c r="F24" s="79"/>
-      <c r="G24" s="79" t="s">
+      <c r="D24" s="102"/>
+      <c r="E24" s="102"/>
+      <c r="F24" s="102"/>
+      <c r="G24" s="102" t="s">
         <v>74</v>
       </c>
-      <c r="H24" s="84"/>
+      <c r="H24" s="99"/>
       <c r="I24" s="16"/>
       <c r="J24" s="16"/>
       <c r="K24" s="16"/>
@@ -5226,16 +5246,16 @@
     <row r="25" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="16"/>
       <c r="B25" s="1"/>
-      <c r="C25" s="80" t="s">
+      <c r="C25" s="105" t="s">
         <v>23</v>
       </c>
-      <c r="D25" s="80"/>
-      <c r="E25" s="80"/>
-      <c r="F25" s="80"/>
-      <c r="G25" s="80" t="s">
+      <c r="D25" s="105"/>
+      <c r="E25" s="105"/>
+      <c r="F25" s="105"/>
+      <c r="G25" s="105" t="s">
         <v>72</v>
       </c>
-      <c r="H25" s="83"/>
+      <c r="H25" s="106"/>
       <c r="I25" s="16"/>
       <c r="J25" s="16"/>
       <c r="K25" s="16"/>
@@ -5247,16 +5267,16 @@
     <row r="26" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="16"/>
       <c r="B26" s="2"/>
-      <c r="C26" s="79" t="s">
+      <c r="C26" s="102" t="s">
         <v>77</v>
       </c>
-      <c r="D26" s="79"/>
-      <c r="E26" s="79"/>
-      <c r="F26" s="79"/>
-      <c r="G26" s="109" t="s">
+      <c r="D26" s="102"/>
+      <c r="E26" s="102"/>
+      <c r="F26" s="102"/>
+      <c r="G26" s="92" t="s">
         <v>78</v>
       </c>
-      <c r="H26" s="110"/>
+      <c r="H26" s="114"/>
       <c r="I26" s="16"/>
       <c r="J26" s="16"/>
       <c r="K26" s="16"/>
@@ -5268,16 +5288,16 @@
     <row r="27" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="16"/>
       <c r="B27" s="1"/>
-      <c r="C27" s="80" t="s">
+      <c r="C27" s="105" t="s">
         <v>70</v>
       </c>
-      <c r="D27" s="80"/>
-      <c r="E27" s="80"/>
-      <c r="F27" s="80"/>
-      <c r="G27" s="130" t="s">
+      <c r="D27" s="105"/>
+      <c r="E27" s="105"/>
+      <c r="F27" s="105"/>
+      <c r="G27" s="163" t="s">
         <v>71</v>
       </c>
-      <c r="H27" s="131"/>
+      <c r="H27" s="164"/>
       <c r="I27" s="16"/>
       <c r="J27" s="16"/>
       <c r="K27" s="16"/>
@@ -5289,16 +5309,16 @@
     <row r="28" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="20"/>
       <c r="B28" s="2"/>
-      <c r="C28" s="79" t="s">
+      <c r="C28" s="102" t="s">
         <v>33</v>
       </c>
-      <c r="D28" s="79"/>
-      <c r="E28" s="79"/>
-      <c r="F28" s="79"/>
-      <c r="G28" s="109" t="s">
+      <c r="D28" s="102"/>
+      <c r="E28" s="102"/>
+      <c r="F28" s="102"/>
+      <c r="G28" s="92" t="s">
         <v>90</v>
       </c>
-      <c r="H28" s="110"/>
+      <c r="H28" s="114"/>
       <c r="I28" s="18"/>
       <c r="J28" s="18"/>
       <c r="K28" s="18"/>
@@ -5310,16 +5330,16 @@
     <row r="29" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="20"/>
       <c r="B29" s="1"/>
-      <c r="C29" s="80" t="s">
+      <c r="C29" s="105" t="s">
         <v>34</v>
       </c>
-      <c r="D29" s="80"/>
-      <c r="E29" s="80"/>
-      <c r="F29" s="80"/>
-      <c r="G29" s="139" t="s">
+      <c r="D29" s="105"/>
+      <c r="E29" s="105"/>
+      <c r="F29" s="105"/>
+      <c r="G29" s="115" t="s">
         <v>35</v>
       </c>
-      <c r="H29" s="83"/>
+      <c r="H29" s="106"/>
       <c r="I29" s="18"/>
       <c r="J29" s="18"/>
       <c r="K29" s="18"/>
@@ -5331,16 +5351,16 @@
     <row r="30" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="20"/>
       <c r="B30" s="2"/>
-      <c r="C30" s="79" t="s">
+      <c r="C30" s="102" t="s">
         <v>36</v>
       </c>
-      <c r="D30" s="79"/>
-      <c r="E30" s="79"/>
-      <c r="F30" s="79"/>
-      <c r="G30" s="121" t="s">
+      <c r="D30" s="102"/>
+      <c r="E30" s="102"/>
+      <c r="F30" s="102"/>
+      <c r="G30" s="133" t="s">
         <v>37</v>
       </c>
-      <c r="H30" s="122"/>
+      <c r="H30" s="134"/>
       <c r="I30" s="18"/>
       <c r="J30" s="18"/>
       <c r="K30" s="18"/>
@@ -5352,16 +5372,16 @@
     <row r="31" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="20"/>
       <c r="B31" s="75"/>
-      <c r="C31" s="125" t="s">
+      <c r="C31" s="100" t="s">
         <v>87</v>
       </c>
-      <c r="D31" s="125"/>
-      <c r="E31" s="125"/>
-      <c r="F31" s="125"/>
-      <c r="G31" s="77" t="s">
+      <c r="D31" s="100"/>
+      <c r="E31" s="100"/>
+      <c r="F31" s="100"/>
+      <c r="G31" s="161" t="s">
         <v>86</v>
       </c>
-      <c r="H31" s="78"/>
+      <c r="H31" s="162"/>
       <c r="I31" s="72"/>
       <c r="J31" s="72"/>
       <c r="K31" s="72"/>
@@ -5373,14 +5393,14 @@
     <row r="32" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="20"/>
       <c r="B32" s="76"/>
-      <c r="C32" s="109" t="s">
+      <c r="C32" s="92" t="s">
         <v>38</v>
       </c>
-      <c r="D32" s="123"/>
-      <c r="E32" s="123"/>
-      <c r="F32" s="124"/>
-      <c r="G32" s="135"/>
-      <c r="H32" s="136"/>
+      <c r="D32" s="93"/>
+      <c r="E32" s="93"/>
+      <c r="F32" s="94"/>
+      <c r="G32" s="110"/>
+      <c r="H32" s="111"/>
       <c r="I32" s="72"/>
       <c r="J32" s="72"/>
       <c r="K32" s="72"/>
@@ -5392,14 +5412,14 @@
     <row r="33" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="20"/>
       <c r="B33" s="75"/>
-      <c r="C33" s="125" t="s">
+      <c r="C33" s="100" t="s">
         <v>40</v>
       </c>
-      <c r="D33" s="125"/>
-      <c r="E33" s="125"/>
-      <c r="F33" s="125"/>
-      <c r="G33" s="137"/>
-      <c r="H33" s="138"/>
+      <c r="D33" s="100"/>
+      <c r="E33" s="100"/>
+      <c r="F33" s="100"/>
+      <c r="G33" s="112"/>
+      <c r="H33" s="113"/>
       <c r="I33" s="18"/>
       <c r="J33" s="18"/>
       <c r="K33" s="18"/>
@@ -5411,14 +5431,14 @@
     <row r="34" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="16"/>
       <c r="B34" s="76"/>
-      <c r="C34" s="79" t="s">
+      <c r="C34" s="102" t="s">
         <v>75</v>
       </c>
-      <c r="D34" s="79"/>
-      <c r="E34" s="79"/>
-      <c r="F34" s="79"/>
-      <c r="G34" s="109"/>
-      <c r="H34" s="110"/>
+      <c r="D34" s="102"/>
+      <c r="E34" s="102"/>
+      <c r="F34" s="102"/>
+      <c r="G34" s="92"/>
+      <c r="H34" s="114"/>
       <c r="I34" s="18"/>
       <c r="J34" s="18"/>
       <c r="K34" s="18"/>
@@ -5429,15 +5449,15 @@
     </row>
     <row r="35" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="20"/>
-      <c r="B35" s="85" t="s">
+      <c r="B35" s="107" t="s">
         <v>65</v>
       </c>
-      <c r="C35" s="86"/>
-      <c r="D35" s="86"/>
-      <c r="E35" s="86"/>
-      <c r="F35" s="86"/>
-      <c r="G35" s="86"/>
-      <c r="H35" s="87"/>
+      <c r="C35" s="108"/>
+      <c r="D35" s="108"/>
+      <c r="E35" s="108"/>
+      <c r="F35" s="108"/>
+      <c r="G35" s="108"/>
+      <c r="H35" s="109"/>
       <c r="I35" s="18"/>
       <c r="J35" s="18"/>
       <c r="K35" s="18"/>
@@ -5448,11 +5468,11 @@
     </row>
     <row r="36" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B36" s="69"/>
-      <c r="C36" s="126" t="s">
+      <c r="C36" s="135" t="s">
         <v>4</v>
       </c>
-      <c r="D36" s="127"/>
-      <c r="E36" s="128"/>
+      <c r="D36" s="136"/>
+      <c r="E36" s="137"/>
       <c r="F36" s="70" t="s">
         <v>5</v>
       </c>
@@ -5469,11 +5489,11 @@
     </row>
     <row r="37" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B37" s="28"/>
-      <c r="C37" s="129" t="s">
+      <c r="C37" s="138" t="s">
         <v>0</v>
       </c>
-      <c r="D37" s="129"/>
-      <c r="E37" s="129"/>
+      <c r="D37" s="138"/>
+      <c r="E37" s="138"/>
       <c r="F37" s="29" t="s">
         <v>15</v>
       </c>
@@ -5490,11 +5510,11 @@
     </row>
     <row r="38" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B38" s="1"/>
-      <c r="C38" s="111" t="s">
+      <c r="C38" s="123" t="s">
         <v>19</v>
       </c>
-      <c r="D38" s="111"/>
-      <c r="E38" s="111"/>
+      <c r="D38" s="123"/>
+      <c r="E38" s="123"/>
       <c r="F38" s="74" t="s">
         <v>112</v>
       </c>
@@ -5512,11 +5532,11 @@
     <row r="39" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="20"/>
       <c r="B39" s="4"/>
-      <c r="C39" s="132" t="s">
+      <c r="C39" s="89" t="s">
         <v>109</v>
       </c>
-      <c r="D39" s="133"/>
-      <c r="E39" s="134"/>
+      <c r="D39" s="90"/>
+      <c r="E39" s="91"/>
       <c r="F39" s="12" t="s">
         <v>113</v>
       </c>
@@ -5537,12 +5557,12 @@
     <row r="40" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="20"/>
       <c r="B40" s="1"/>
-      <c r="C40" s="111" t="s">
+      <c r="C40" s="123" t="s">
         <v>123</v>
       </c>
-      <c r="D40" s="111"/>
-      <c r="E40" s="111"/>
-      <c r="F40" s="165" t="s">
+      <c r="D40" s="123"/>
+      <c r="E40" s="123"/>
+      <c r="F40" s="81" t="s">
         <v>124</v>
       </c>
       <c r="G40" s="74" t="s">
@@ -5561,18 +5581,18 @@
     </row>
     <row r="41" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B41" s="4"/>
-      <c r="C41" s="167" t="s">
+      <c r="C41" s="119" t="s">
         <v>91</v>
       </c>
-      <c r="D41" s="167"/>
-      <c r="E41" s="167"/>
+      <c r="D41" s="119"/>
+      <c r="E41" s="119"/>
       <c r="F41" s="12" t="s">
         <v>121</v>
       </c>
       <c r="G41" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="H41" s="168" t="s">
+      <c r="H41" s="83" t="s">
         <v>104</v>
       </c>
       <c r="I41" s="18"/>
@@ -5581,19 +5601,19 @@
       <c r="L41" s="18"/>
     </row>
     <row r="42" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B42" s="158"/>
-      <c r="C42" s="164" t="s">
+      <c r="B42" s="78"/>
+      <c r="C42" s="120" t="s">
         <v>98</v>
       </c>
-      <c r="D42" s="164"/>
-      <c r="E42" s="164"/>
-      <c r="F42" s="162" t="s">
+      <c r="D42" s="120"/>
+      <c r="E42" s="120"/>
+      <c r="F42" s="79" t="s">
         <v>114</v>
       </c>
-      <c r="G42" s="165" t="s">
+      <c r="G42" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="H42" s="163" t="s">
+      <c r="H42" s="80" t="s">
         <v>99</v>
       </c>
       <c r="I42" s="3"/>
@@ -5602,18 +5622,18 @@
     </row>
     <row r="43" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B43" s="4"/>
-      <c r="C43" s="167" t="s">
+      <c r="C43" s="119" t="s">
         <v>97</v>
       </c>
-      <c r="D43" s="167"/>
-      <c r="E43" s="167"/>
+      <c r="D43" s="119"/>
+      <c r="E43" s="119"/>
       <c r="F43" s="12" t="s">
         <v>115</v>
       </c>
       <c r="G43" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="H43" s="168" t="s">
+      <c r="H43" s="83" t="s">
         <v>100</v>
       </c>
       <c r="I43" s="3"/>
@@ -5621,19 +5641,19 @@
       <c r="L43" s="18"/>
     </row>
     <row r="44" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B44" s="158"/>
-      <c r="C44" s="164" t="s">
+      <c r="B44" s="78"/>
+      <c r="C44" s="120" t="s">
         <v>96</v>
       </c>
-      <c r="D44" s="164"/>
-      <c r="E44" s="164"/>
-      <c r="F44" s="162" t="s">
+      <c r="D44" s="120"/>
+      <c r="E44" s="120"/>
+      <c r="F44" s="79" t="s">
         <v>116</v>
       </c>
-      <c r="G44" s="165" t="s">
+      <c r="G44" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="H44" s="163" t="s">
+      <c r="H44" s="80" t="s">
         <v>107</v>
       </c>
       <c r="I44" s="3"/>
@@ -5642,18 +5662,18 @@
     </row>
     <row r="45" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B45" s="4"/>
-      <c r="C45" s="167" t="s">
+      <c r="C45" s="119" t="s">
         <v>95</v>
       </c>
-      <c r="D45" s="167"/>
-      <c r="E45" s="167"/>
+      <c r="D45" s="119"/>
+      <c r="E45" s="119"/>
       <c r="F45" s="12" t="s">
         <v>117</v>
       </c>
       <c r="G45" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="H45" s="168" t="s">
+      <c r="H45" s="83" t="s">
         <v>108</v>
       </c>
       <c r="I45" s="3"/>
@@ -5661,55 +5681,55 @@
       <c r="L45" s="18"/>
     </row>
     <row r="46" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B46" s="158"/>
-      <c r="C46" s="164" t="s">
+      <c r="B46" s="78"/>
+      <c r="C46" s="120" t="s">
         <v>94</v>
       </c>
-      <c r="D46" s="164"/>
-      <c r="E46" s="164"/>
-      <c r="F46" s="162" t="s">
+      <c r="D46" s="120"/>
+      <c r="E46" s="120"/>
+      <c r="F46" s="79" t="s">
         <v>118</v>
       </c>
-      <c r="G46" s="165" t="s">
+      <c r="G46" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="H46" s="163" t="s">
+      <c r="H46" s="80" t="s">
         <v>101</v>
       </c>
       <c r="I46" s="3"/>
     </row>
     <row r="47" spans="1:15" x14ac:dyDescent="0.3">
       <c r="B47" s="4"/>
-      <c r="C47" s="167" t="s">
+      <c r="C47" s="119" t="s">
         <v>93</v>
       </c>
-      <c r="D47" s="167"/>
-      <c r="E47" s="167"/>
+      <c r="D47" s="119"/>
+      <c r="E47" s="119"/>
       <c r="F47" s="12" t="s">
         <v>119</v>
       </c>
       <c r="G47" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="H47" s="168" t="s">
+      <c r="H47" s="83" t="s">
         <v>102</v>
       </c>
       <c r="I47" s="3"/>
     </row>
     <row r="48" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B48" s="158"/>
-      <c r="C48" s="164" t="s">
+      <c r="B48" s="78"/>
+      <c r="C48" s="120" t="s">
         <v>92</v>
       </c>
-      <c r="D48" s="164"/>
-      <c r="E48" s="164"/>
-      <c r="F48" s="162" t="s">
+      <c r="D48" s="120"/>
+      <c r="E48" s="120"/>
+      <c r="F48" s="79" t="s">
         <v>122</v>
       </c>
-      <c r="G48" s="165" t="s">
+      <c r="G48" s="81" t="s">
         <v>20</v>
       </c>
-      <c r="H48" s="163" t="s">
+      <c r="H48" s="80" t="s">
         <v>103</v>
       </c>
       <c r="I48" s="3"/>
@@ -5717,15 +5737,15 @@
     <row r="49" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="20"/>
       <c r="B49" s="76"/>
-      <c r="C49" s="156" t="s">
+      <c r="C49" s="157" t="s">
         <v>105</v>
       </c>
-      <c r="D49" s="156"/>
-      <c r="E49" s="156"/>
-      <c r="F49" s="157" t="s">
+      <c r="D49" s="157"/>
+      <c r="E49" s="157"/>
+      <c r="F49" s="77" t="s">
         <v>120</v>
       </c>
-      <c r="G49" s="157" t="s">
+      <c r="G49" s="77" t="s">
         <v>20</v>
       </c>
       <c r="H49" s="10" t="s">
@@ -5740,60 +5760,60 @@
       <c r="O49" s="20"/>
     </row>
     <row r="50" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B50" s="158"/>
-      <c r="C50" s="159" t="s">
+      <c r="B50" s="78"/>
+      <c r="C50" s="116" t="s">
         <v>10</v>
       </c>
-      <c r="D50" s="160"/>
-      <c r="E50" s="161"/>
-      <c r="F50" s="162" t="s">
+      <c r="D50" s="117"/>
+      <c r="E50" s="118"/>
+      <c r="F50" s="79" t="s">
         <v>125</v>
       </c>
-      <c r="G50" s="162" t="s">
+      <c r="G50" s="79" t="s">
         <v>11</v>
       </c>
-      <c r="H50" s="166" t="s">
+      <c r="H50" s="82" t="s">
         <v>12</v>
       </c>
       <c r="I50" s="3"/>
     </row>
     <row r="51" spans="1:15" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B51" s="4"/>
-      <c r="C51" s="132" t="s">
+      <c r="C51" s="89" t="s">
         <v>68</v>
       </c>
-      <c r="D51" s="133"/>
-      <c r="E51" s="134"/>
+      <c r="D51" s="90"/>
+      <c r="E51" s="91"/>
       <c r="F51" s="12" t="s">
         <v>69</v>
       </c>
       <c r="G51" s="13" t="s">
         <v>8</v>
       </c>
-      <c r="H51" s="168"/>
+      <c r="H51" s="83"/>
       <c r="I51" s="3"/>
     </row>
     <row r="52" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="B52" s="112" t="s">
+      <c r="B52" s="124" t="s">
         <v>67</v>
       </c>
-      <c r="C52" s="113"/>
-      <c r="D52" s="113"/>
-      <c r="E52" s="113"/>
-      <c r="F52" s="113"/>
-      <c r="G52" s="113"/>
-      <c r="H52" s="114"/>
+      <c r="C52" s="125"/>
+      <c r="D52" s="125"/>
+      <c r="E52" s="125"/>
+      <c r="F52" s="125"/>
+      <c r="G52" s="125"/>
+      <c r="H52" s="126"/>
       <c r="I52" s="3"/>
     </row>
     <row r="53" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A53" s="9"/>
-      <c r="B53" s="115"/>
-      <c r="C53" s="116"/>
-      <c r="D53" s="116"/>
-      <c r="E53" s="116"/>
-      <c r="F53" s="116"/>
-      <c r="G53" s="116"/>
-      <c r="H53" s="117"/>
+      <c r="B53" s="127"/>
+      <c r="C53" s="128"/>
+      <c r="D53" s="128"/>
+      <c r="E53" s="128"/>
+      <c r="F53" s="128"/>
+      <c r="G53" s="128"/>
+      <c r="H53" s="129"/>
       <c r="I53" s="3"/>
       <c r="J53" s="9"/>
       <c r="K53" s="9"/>
@@ -5804,13 +5824,13 @@
     </row>
     <row r="54" spans="1:15" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A54" s="9"/>
-      <c r="B54" s="115"/>
-      <c r="C54" s="116"/>
-      <c r="D54" s="116"/>
-      <c r="E54" s="116"/>
-      <c r="F54" s="116"/>
-      <c r="G54" s="116"/>
-      <c r="H54" s="117"/>
+      <c r="B54" s="127"/>
+      <c r="C54" s="128"/>
+      <c r="D54" s="128"/>
+      <c r="E54" s="128"/>
+      <c r="F54" s="128"/>
+      <c r="G54" s="128"/>
+      <c r="H54" s="129"/>
       <c r="I54" s="15"/>
       <c r="J54" s="9"/>
       <c r="K54" s="9"/>
@@ -5821,13 +5841,13 @@
     </row>
     <row r="55" spans="1:15" s="8" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="9"/>
-      <c r="B55" s="118"/>
-      <c r="C55" s="119"/>
-      <c r="D55" s="119"/>
-      <c r="E55" s="119"/>
-      <c r="F55" s="119"/>
-      <c r="G55" s="119"/>
-      <c r="H55" s="120"/>
+      <c r="B55" s="130"/>
+      <c r="C55" s="131"/>
+      <c r="D55" s="131"/>
+      <c r="E55" s="131"/>
+      <c r="F55" s="131"/>
+      <c r="G55" s="131"/>
+      <c r="H55" s="132"/>
       <c r="I55" s="15"/>
       <c r="J55" s="9"/>
       <c r="K55" s="9"/>
@@ -5859,8 +5879,8 @@
       <c r="D57" s="17"/>
       <c r="E57" s="17"/>
       <c r="F57" s="17"/>
-      <c r="G57" s="93"/>
-      <c r="H57" s="93"/>
+      <c r="G57" s="122"/>
+      <c r="H57" s="122"/>
       <c r="I57" s="15"/>
     </row>
     <row r="58" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5869,8 +5889,8 @@
       <c r="D58" s="17"/>
       <c r="E58" s="17"/>
       <c r="F58" s="17"/>
-      <c r="G58" s="93"/>
-      <c r="H58" s="93"/>
+      <c r="G58" s="122"/>
+      <c r="H58" s="122"/>
       <c r="I58" s="15"/>
     </row>
     <row r="59" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -5879,14 +5899,14 @@
       <c r="D59" s="17"/>
       <c r="E59" s="17"/>
       <c r="F59" s="17"/>
-      <c r="G59" s="93"/>
-      <c r="H59" s="93"/>
+      <c r="G59" s="122"/>
+      <c r="H59" s="122"/>
     </row>
     <row r="60" spans="1:15" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B60" s="93"/>
-      <c r="C60" s="93"/>
-      <c r="D60" s="93"/>
-      <c r="E60" s="93"/>
+      <c r="B60" s="122"/>
+      <c r="C60" s="122"/>
+      <c r="D60" s="122"/>
+      <c r="E60" s="122"/>
       <c r="F60" s="17"/>
       <c r="G60" s="17"/>
       <c r="H60" s="17"/>
@@ -6035,9 +6055,9 @@
     </row>
     <row r="87" spans="1:10" s="9" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B87" s="17"/>
-      <c r="C87" s="91"/>
-      <c r="D87" s="91"/>
-      <c r="E87" s="91"/>
+      <c r="C87" s="121"/>
+      <c r="D87" s="121"/>
+      <c r="E87" s="121"/>
       <c r="F87" s="17"/>
       <c r="G87" s="17"/>
       <c r="H87" s="17"/>
@@ -8258,49 +8278,28 @@
     </row>
   </sheetData>
   <mergeCells count="81">
-    <mergeCell ref="C39:E39"/>
-    <mergeCell ref="C8:F8"/>
-    <mergeCell ref="C9:F9"/>
-    <mergeCell ref="C10:F10"/>
-    <mergeCell ref="C11:F11"/>
-    <mergeCell ref="C12:F12"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="G18:H18"/>
-    <mergeCell ref="G17:H17"/>
-    <mergeCell ref="G15:H15"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="G16:H16"/>
-    <mergeCell ref="B35:H35"/>
-    <mergeCell ref="G32:H32"/>
-    <mergeCell ref="G33:H33"/>
-    <mergeCell ref="G34:H34"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="C30:F30"/>
-    <mergeCell ref="C51:E51"/>
-    <mergeCell ref="C50:E50"/>
-    <mergeCell ref="C45:E45"/>
-    <mergeCell ref="C46:E46"/>
-    <mergeCell ref="C47:E47"/>
-    <mergeCell ref="C48:E48"/>
-    <mergeCell ref="C34:F34"/>
-    <mergeCell ref="C28:F28"/>
-    <mergeCell ref="C29:F29"/>
-    <mergeCell ref="C87:E87"/>
-    <mergeCell ref="B60:E60"/>
-    <mergeCell ref="C38:E38"/>
-    <mergeCell ref="C41:E41"/>
-    <mergeCell ref="C40:E40"/>
-    <mergeCell ref="B52:H55"/>
-    <mergeCell ref="G30:H30"/>
-    <mergeCell ref="C32:F32"/>
-    <mergeCell ref="C33:F33"/>
-    <mergeCell ref="C36:E36"/>
-    <mergeCell ref="C37:E37"/>
-    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="G31:H31"/>
+    <mergeCell ref="C26:F26"/>
+    <mergeCell ref="C22:F22"/>
+    <mergeCell ref="C23:F23"/>
+    <mergeCell ref="C24:F24"/>
+    <mergeCell ref="C25:F25"/>
+    <mergeCell ref="C27:F27"/>
+    <mergeCell ref="G26:H26"/>
+    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="C15:F15"/>
+    <mergeCell ref="G25:H25"/>
+    <mergeCell ref="G22:H22"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="G24:H24"/>
+    <mergeCell ref="C20:F20"/>
+    <mergeCell ref="C21:F21"/>
+    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="G21:H21"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="C17:F17"/>
+    <mergeCell ref="B19:H19"/>
+    <mergeCell ref="B8:B18"/>
     <mergeCell ref="G2:H5"/>
     <mergeCell ref="G57:H59"/>
     <mergeCell ref="B2:D2"/>
@@ -8317,28 +8316,49 @@
     <mergeCell ref="C18:F18"/>
     <mergeCell ref="C13:H13"/>
     <mergeCell ref="C14:F14"/>
-    <mergeCell ref="C15:F15"/>
-    <mergeCell ref="G25:H25"/>
-    <mergeCell ref="G22:H22"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="G24:H24"/>
-    <mergeCell ref="C20:F20"/>
-    <mergeCell ref="C21:F21"/>
-    <mergeCell ref="G20:H20"/>
-    <mergeCell ref="G21:H21"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="C17:F17"/>
-    <mergeCell ref="B19:H19"/>
-    <mergeCell ref="B8:B18"/>
-    <mergeCell ref="G31:H31"/>
-    <mergeCell ref="C26:F26"/>
-    <mergeCell ref="C22:F22"/>
-    <mergeCell ref="C23:F23"/>
-    <mergeCell ref="C24:F24"/>
-    <mergeCell ref="C25:F25"/>
-    <mergeCell ref="C27:F27"/>
-    <mergeCell ref="G26:H26"/>
-    <mergeCell ref="G27:H27"/>
+    <mergeCell ref="C32:F32"/>
+    <mergeCell ref="C33:F33"/>
+    <mergeCell ref="C36:E36"/>
+    <mergeCell ref="C37:E37"/>
+    <mergeCell ref="C31:F31"/>
+    <mergeCell ref="C87:E87"/>
+    <mergeCell ref="B60:E60"/>
+    <mergeCell ref="C38:E38"/>
+    <mergeCell ref="C41:E41"/>
+    <mergeCell ref="C40:E40"/>
+    <mergeCell ref="B52:H55"/>
+    <mergeCell ref="C51:E51"/>
+    <mergeCell ref="C50:E50"/>
+    <mergeCell ref="C45:E45"/>
+    <mergeCell ref="C46:E46"/>
+    <mergeCell ref="C47:E47"/>
+    <mergeCell ref="C48:E48"/>
+    <mergeCell ref="G18:H18"/>
+    <mergeCell ref="G17:H17"/>
+    <mergeCell ref="G15:H15"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="G16:H16"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="C39:E39"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="C10:F10"/>
+    <mergeCell ref="C11:F11"/>
+    <mergeCell ref="C12:F12"/>
+    <mergeCell ref="B35:H35"/>
+    <mergeCell ref="G32:H32"/>
+    <mergeCell ref="G33:H33"/>
+    <mergeCell ref="G34:H34"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="C30:F30"/>
+    <mergeCell ref="C34:F34"/>
+    <mergeCell ref="C28:F28"/>
+    <mergeCell ref="C29:F29"/>
+    <mergeCell ref="G30:H30"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="G18:H18" location="'Stack-up'!A1" display="See "/>
@@ -9243,7 +9263,7 @@
   </sheetPr>
   <dimension ref="C2:U25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
@@ -9267,9 +9287,9 @@
       <c r="G2" s="7" t="s">
         <v>42</v>
       </c>
-      <c r="S2" s="147"/>
-      <c r="T2" s="147"/>
-      <c r="U2" s="147"/>
+      <c r="S2" s="172"/>
+      <c r="T2" s="172"/>
+      <c r="U2" s="172"/>
     </row>
     <row r="3" spans="3:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C3" s="42" t="s">
@@ -9287,9 +9307,9 @@
       </c>
       <c r="H3" s="59"/>
       <c r="I3" s="32"/>
-      <c r="S3" s="150"/>
-      <c r="T3" s="150"/>
-      <c r="U3" s="150"/>
+      <c r="S3" s="173"/>
+      <c r="T3" s="173"/>
+      <c r="U3" s="173"/>
     </row>
     <row r="4" spans="3:21" x14ac:dyDescent="0.3">
       <c r="C4" s="49"/>
@@ -9299,16 +9319,16 @@
       <c r="E4" s="51">
         <v>48</v>
       </c>
-      <c r="F4" s="148">
+      <c r="F4" s="165">
         <f>E4+E5</f>
         <v>96</v>
       </c>
       <c r="G4" s="52"/>
       <c r="H4" s="60"/>
       <c r="I4" s="32"/>
-      <c r="S4" s="150"/>
-      <c r="T4" s="150"/>
-      <c r="U4" s="150"/>
+      <c r="S4" s="173"/>
+      <c r="T4" s="173"/>
+      <c r="U4" s="173"/>
     </row>
     <row r="5" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C5" s="53"/>
@@ -9318,7 +9338,7 @@
       <c r="E5" s="55">
         <v>48</v>
       </c>
-      <c r="F5" s="149"/>
+      <c r="F5" s="166"/>
       <c r="G5" s="56"/>
       <c r="H5" s="61"/>
       <c r="I5" s="32"/>
@@ -9328,9 +9348,9 @@
       <c r="Q5" s="7">
         <v>25.4</v>
       </c>
-      <c r="S5" s="150"/>
-      <c r="T5" s="150"/>
-      <c r="U5" s="150"/>
+      <c r="S5" s="173"/>
+      <c r="T5" s="173"/>
+      <c r="U5" s="173"/>
     </row>
     <row r="6" spans="3:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C6" s="42" t="s">
@@ -9348,9 +9368,9 @@
       </c>
       <c r="H6" s="62"/>
       <c r="I6" s="33"/>
-      <c r="S6" s="150"/>
-      <c r="T6" s="150"/>
-      <c r="U6" s="150"/>
+      <c r="S6" s="173"/>
+      <c r="T6" s="173"/>
+      <c r="U6" s="173"/>
     </row>
     <row r="7" spans="3:21" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C7" s="49"/>
@@ -9360,7 +9380,7 @@
       <c r="E7" s="57">
         <v>48</v>
       </c>
-      <c r="F7" s="151">
+      <c r="F7" s="171">
         <f>E7+E8</f>
         <v>149.6</v>
       </c>
@@ -9380,7 +9400,7 @@
         <f>Q8</f>
         <v>101.6</v>
       </c>
-      <c r="F8" s="151"/>
+      <c r="F8" s="171"/>
       <c r="G8" s="38"/>
       <c r="H8" s="64"/>
       <c r="I8" s="34"/>
@@ -9424,7 +9444,7 @@
       <c r="E10" s="51">
         <v>71</v>
       </c>
-      <c r="F10" s="148">
+      <c r="F10" s="165">
         <f>E10+E11</f>
         <v>142</v>
       </c>
@@ -9447,7 +9467,7 @@
       <c r="E11" s="55">
         <v>71</v>
       </c>
-      <c r="F11" s="149"/>
+      <c r="F11" s="166"/>
       <c r="G11" s="56"/>
       <c r="H11" s="66"/>
       <c r="I11" s="34"/>
@@ -9486,16 +9506,16 @@
       </c>
     </row>
     <row r="13" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C13" s="169"/>
-      <c r="D13" s="170" t="s">
+      <c r="C13" s="84"/>
+      <c r="D13" s="85" t="s">
         <v>110</v>
       </c>
-      <c r="E13" s="171">
+      <c r="E13" s="86">
         <v>50</v>
       </c>
-      <c r="F13" s="172"/>
-      <c r="G13" s="170"/>
-      <c r="H13" s="173"/>
+      <c r="F13" s="87"/>
+      <c r="G13" s="85"/>
+      <c r="H13" s="88"/>
       <c r="I13" s="34"/>
     </row>
     <row r="14" spans="3:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
@@ -9525,7 +9545,7 @@
       <c r="E15" s="51">
         <v>71</v>
       </c>
-      <c r="F15" s="148">
+      <c r="F15" s="165">
         <f>E15+E16</f>
         <v>142</v>
       </c>
@@ -9541,7 +9561,7 @@
       <c r="E16" s="55">
         <v>71</v>
       </c>
-      <c r="F16" s="149"/>
+      <c r="F16" s="166"/>
       <c r="G16" s="56"/>
       <c r="H16" s="66"/>
       <c r="I16" s="34"/>
@@ -9574,7 +9594,7 @@
         <f>Q8</f>
         <v>101.6</v>
       </c>
-      <c r="F18" s="151">
+      <c r="F18" s="171">
         <f>E18+E19</f>
         <v>149.6</v>
       </c>
@@ -9590,7 +9610,7 @@
       <c r="E19" s="57">
         <v>48</v>
       </c>
-      <c r="F19" s="151"/>
+      <c r="F19" s="171"/>
       <c r="G19" s="58"/>
       <c r="H19" s="63"/>
       <c r="I19" s="34"/>
@@ -9620,7 +9640,7 @@
       <c r="E21" s="51">
         <v>48</v>
       </c>
-      <c r="F21" s="148">
+      <c r="F21" s="165">
         <f>E21+E22</f>
         <v>96</v>
       </c>
@@ -9636,7 +9656,7 @@
       <c r="E22" s="55">
         <v>48</v>
       </c>
-      <c r="F22" s="149"/>
+      <c r="F22" s="166"/>
       <c r="G22" s="56"/>
       <c r="H22" s="61"/>
       <c r="I22" s="34"/>
@@ -9668,15 +9688,15 @@
       <c r="I24" s="40"/>
     </row>
     <row r="25" spans="3:9" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C25" s="154" t="s">
+      <c r="C25" s="169" t="s">
         <v>63</v>
       </c>
-      <c r="D25" s="155"/>
-      <c r="E25" s="152">
+      <c r="D25" s="170"/>
+      <c r="E25" s="167">
         <f>SUM(E3:E23)</f>
         <v>997.2</v>
       </c>
-      <c r="F25" s="153"/>
+      <c r="F25" s="168"/>
       <c r="G25" s="26"/>
       <c r="H25" s="41"/>
       <c r="I25" s="40"/>

</xml_diff>